<commit_message>
some of severn cases have been modeled again
</commit_message>
<xml_diff>
--- a/archived modeled files/Severn River/Raw and un-modeled excel files to be run by WATUM/Dx_1975_Fischer_paper02_severn.xlsx
+++ b/archived modeled files/Severn River/Raw and un-modeled excel files to be run by WATUM/Dx_1975_Fischer_paper02_severn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="8" r:id="rId1"/>
@@ -1672,15 +1672,6 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="7" xfId="37" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1705,6 +1696,15 @@
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -4686,7 +4686,7 @@
   <dimension ref="A1:X91"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4850,7 +4850,7 @@
       </c>
       <c r="B6" s="51" t="str">
         <f ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"),1)-1)</f>
-        <v>C:\Users\Mostafa\Desktop\watum_Working_Branch\archived modeled files\Severn River\Raw and un-modeled excel files to be run by WATUM\</v>
+        <v>C:\Users\Mostafa\Desktop\watum_Working_Branch\</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -4964,7 +4964,7 @@
         <v>30</v>
       </c>
       <c r="B10" s="53">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -7347,7 +7347,7 @@
       </c>
       <c r="AB2" s="78">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="AC2" s="78">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7359,7 +7359,7 @@
       </c>
       <c r="AE2" s="76">
         <f t="shared" ref="AE2:AE3" si="0">Delta_T__seconds</f>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="AF2" s="77">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7491,7 +7491,7 @@
       </c>
       <c r="AB3" s="78">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>77</v>
+        <v>222</v>
       </c>
       <c r="AC3" s="78">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7503,7 +7503,7 @@
       </c>
       <c r="AE3" s="76">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="AF3" s="77">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7635,7 +7635,7 @@
       </c>
       <c r="AB4" s="85">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>203</v>
+        <v>582</v>
       </c>
       <c r="AC4" s="85">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7647,7 +7647,7 @@
       </c>
       <c r="AE4" s="76">
         <f>Delta_T__seconds</f>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="AF4" s="77">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7775,7 +7775,7 @@
       </c>
       <c r="AB5" s="85">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>444</v>
+        <v>1268</v>
       </c>
       <c r="AC5" s="85">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7787,7 +7787,7 @@
       </c>
       <c r="AE5" s="76">
         <f>Delta_T__seconds</f>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="AF5" s="77">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7915,7 +7915,7 @@
       </c>
       <c r="AB6" s="85">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>671</v>
+        <v>1919</v>
       </c>
       <c r="AC6" s="85">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7927,7 +7927,7 @@
       </c>
       <c r="AE6" s="76">
         <f>Delta_T__seconds</f>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="AF6" s="77">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8055,7 +8055,7 @@
       </c>
       <c r="AB7" s="85">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>905</v>
+        <v>2588</v>
       </c>
       <c r="AC7" s="85">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -8067,7 +8067,7 @@
       </c>
       <c r="AE7" s="76">
         <f>Delta_T__seconds</f>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="AF7" s="77">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8195,7 +8195,7 @@
       </c>
       <c r="AB8" s="85">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>1176</v>
+        <v>3361</v>
       </c>
       <c r="AC8" s="85">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -8207,7 +8207,7 @@
       </c>
       <c r="AE8" s="76">
         <f>Delta_T__seconds</f>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="AF8" s="77">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8363,7 +8363,7 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -8473,16 +8473,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" style="109"/>
-    <col min="14" max="14" width="47.140625" style="112" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="109"/>
+    <col min="12" max="13" width="9.140625" style="106"/>
+    <col min="14" max="14" width="47.140625" style="109" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="106"/>
     <col min="16" max="16" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8491,15 +8491,15 @@
       <c r="H1">
         <v>1</v>
       </c>
-      <c r="N1" s="110"/>
+      <c r="N1" s="107"/>
     </row>
     <row r="2" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
       <c r="H2">
         <v>5</v>
       </c>
-      <c r="N2" s="111"/>
-      <c r="P2" s="106" t="s">
+      <c r="N2" s="108"/>
+      <c r="P2" s="103" t="s">
         <v>108</v>
       </c>
     </row>
@@ -8508,8 +8508,8 @@
       <c r="H3">
         <v>10</v>
       </c>
-      <c r="N3" s="111"/>
-      <c r="P3" s="107" t="s">
+      <c r="N3" s="108"/>
+      <c r="P3" s="104" t="s">
         <v>85</v>
       </c>
     </row>
@@ -8518,8 +8518,8 @@
       <c r="H4">
         <v>25</v>
       </c>
-      <c r="N4" s="111"/>
-      <c r="P4" s="107" t="s">
+      <c r="N4" s="108"/>
+      <c r="P4" s="104" t="s">
         <v>86</v>
       </c>
     </row>
@@ -8528,8 +8528,8 @@
       <c r="H5">
         <v>50</v>
       </c>
-      <c r="N5" s="111"/>
-      <c r="P5" s="107" t="s">
+      <c r="N5" s="108"/>
+      <c r="P5" s="104" t="s">
         <v>87</v>
       </c>
     </row>
@@ -8538,8 +8538,8 @@
       <c r="H6">
         <v>100</v>
       </c>
-      <c r="N6" s="111"/>
-      <c r="P6" s="107" t="s">
+      <c r="N6" s="108"/>
+      <c r="P6" s="104" t="s">
         <v>88</v>
       </c>
     </row>
@@ -8548,8 +8548,8 @@
       <c r="H7">
         <v>150</v>
       </c>
-      <c r="N7" s="111"/>
-      <c r="P7" s="107" t="s">
+      <c r="N7" s="108"/>
+      <c r="P7" s="104" t="s">
         <v>89</v>
       </c>
     </row>
@@ -8558,8 +8558,8 @@
       <c r="H8">
         <v>200</v>
       </c>
-      <c r="N8" s="111"/>
-      <c r="P8" s="107" t="s">
+      <c r="N8" s="108"/>
+      <c r="P8" s="104" t="s">
         <v>90</v>
       </c>
     </row>
@@ -8568,8 +8568,8 @@
       <c r="H9">
         <v>250</v>
       </c>
-      <c r="N9" s="111"/>
-      <c r="P9" s="107" t="s">
+      <c r="N9" s="108"/>
+      <c r="P9" s="104" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8578,8 +8578,8 @@
       <c r="H10">
         <v>300</v>
       </c>
-      <c r="N10" s="111"/>
-      <c r="P10" s="107" t="s">
+      <c r="N10" s="108"/>
+      <c r="P10" s="104" t="s">
         <v>92</v>
       </c>
     </row>
@@ -8587,8 +8587,8 @@
       <c r="H11">
         <v>350</v>
       </c>
-      <c r="N11" s="111"/>
-      <c r="P11" s="107" t="s">
+      <c r="N11" s="108"/>
+      <c r="P11" s="104" t="s">
         <v>109</v>
       </c>
     </row>
@@ -8596,8 +8596,8 @@
       <c r="H12">
         <v>400</v>
       </c>
-      <c r="N12" s="111"/>
-      <c r="P12" s="108" t="s">
+      <c r="N12" s="108"/>
+      <c r="P12" s="105" t="s">
         <v>110</v>
       </c>
     </row>
@@ -8605,8 +8605,8 @@
       <c r="H13">
         <v>450</v>
       </c>
-      <c r="N13" s="111"/>
-      <c r="P13" s="107" t="s">
+      <c r="N13" s="108"/>
+      <c r="P13" s="104" t="s">
         <v>111</v>
       </c>
     </row>
@@ -8614,8 +8614,8 @@
       <c r="H14">
         <v>500</v>
       </c>
-      <c r="N14" s="111"/>
-      <c r="P14" s="107" t="s">
+      <c r="N14" s="108"/>
+      <c r="P14" s="104" t="s">
         <v>93</v>
       </c>
     </row>
@@ -8623,8 +8623,8 @@
       <c r="H15">
         <v>550</v>
       </c>
-      <c r="N15" s="111"/>
-      <c r="P15" s="107" t="s">
+      <c r="N15" s="108"/>
+      <c r="P15" s="104" t="s">
         <v>94</v>
       </c>
     </row>
@@ -8632,8 +8632,8 @@
       <c r="H16">
         <v>600</v>
       </c>
-      <c r="N16" s="111"/>
-      <c r="P16" s="107" t="s">
+      <c r="N16" s="108"/>
+      <c r="P16" s="104" t="s">
         <v>95</v>
       </c>
     </row>
@@ -8641,8 +8641,8 @@
       <c r="H17">
         <v>650</v>
       </c>
-      <c r="N17" s="111"/>
-      <c r="P17" s="107" t="s">
+      <c r="N17" s="108"/>
+      <c r="P17" s="104" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8650,8 +8650,8 @@
       <c r="H18">
         <v>700</v>
       </c>
-      <c r="N18" s="111"/>
-      <c r="P18" s="107" t="s">
+      <c r="N18" s="108"/>
+      <c r="P18" s="104" t="s">
         <v>97</v>
       </c>
     </row>
@@ -8659,8 +8659,8 @@
       <c r="H19">
         <v>750</v>
       </c>
-      <c r="N19" s="111"/>
-      <c r="P19" s="107" t="s">
+      <c r="N19" s="108"/>
+      <c r="P19" s="104" t="s">
         <v>98</v>
       </c>
     </row>
@@ -8668,7 +8668,7 @@
       <c r="H20">
         <v>800</v>
       </c>
-      <c r="P20" s="107" t="s">
+      <c r="P20" s="104" t="s">
         <v>112</v>
       </c>
     </row>
@@ -8676,7 +8676,7 @@
       <c r="H21">
         <v>900</v>
       </c>
-      <c r="P21" s="107" t="s">
+      <c r="P21" s="104" t="s">
         <v>113</v>
       </c>
     </row>
@@ -8684,7 +8684,7 @@
       <c r="H22">
         <v>1000</v>
       </c>
-      <c r="P22" s="105" t="s">
+      <c r="P22" s="102" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8692,7 +8692,7 @@
       <c r="H23">
         <v>1250</v>
       </c>
-      <c r="N23" s="113"/>
+      <c r="N23" s="110"/>
     </row>
     <row r="24" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H24">
@@ -8730,7 +8730,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I7"/>
+      <selection activeCell="A2" sqref="A2:S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8766,131 +8766,238 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.31322849740396147</v>
+        <v>0.68015664268852827</v>
       </c>
       <c r="B2">
-        <v>36.525382552168367</v>
+        <v>28625.050200190482</v>
       </c>
       <c r="C2">
-        <v>32.534000789767745</v>
+        <v>7.5719455818316364E-2</v>
       </c>
       <c r="D2">
-        <v>33.417506117698331</v>
+        <v>14.381730614658528</v>
       </c>
       <c r="E2">
-        <v>38.84840735065351</v>
+        <v>8397713719.6893826</v>
       </c>
       <c r="F2">
-        <v>23.277590695310806</v>
+        <v>16659637699.36138</v>
       </c>
       <c r="G2">
-        <v>34.811568463568335</v>
+        <v>53.346954629423969</v>
       </c>
       <c r="H2">
-        <v>32.643688089241856</v>
+        <v>24.944368285190407</v>
       </c>
       <c r="I2">
-        <v>20.812053037658316</v>
+        <v>8.9633660700929063</v>
+      </c>
+      <c r="J2">
+        <v>1.7314104976385134</v>
+      </c>
+      <c r="K2">
+        <v>27.52928439270714</v>
+      </c>
+      <c r="L2">
+        <v>15.313694228549927</v>
+      </c>
+      <c r="M2">
+        <v>41.108331001401368</v>
+      </c>
+      <c r="N2">
+        <v>27.453400050271661</v>
+      </c>
+      <c r="O2">
+        <v>5.4214850129549559</v>
+      </c>
+      <c r="P2">
+        <v>35.884936034862996</v>
+      </c>
+      <c r="Q2">
+        <v>9.014130288461315</v>
+      </c>
+      <c r="R2">
+        <v>21.676550151409781</v>
+      </c>
+      <c r="S2">
+        <v>13.942155495606716</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.26698111766955995</v>
+        <v>0.31322849740396147</v>
       </c>
       <c r="B3">
-        <v>33.390806589551822</v>
+        <v>68852.677170974173</v>
       </c>
       <c r="C3">
-        <v>14.03880466851562</v>
+        <v>0.12293688374554616</v>
       </c>
       <c r="D3">
-        <v>43.206819882737427</v>
+        <v>36.525382552168367</v>
       </c>
       <c r="E3">
-        <v>45.241875502440102</v>
+        <v>1191998690413.3914</v>
       </c>
       <c r="F3">
-        <v>41.63305266191491</v>
+        <v>1694556080269.5063</v>
       </c>
       <c r="G3">
-        <v>35.359440679528277</v>
+        <v>32.534000789767745</v>
       </c>
       <c r="H3">
-        <v>31.962756249979922</v>
+        <v>33.417506117698331</v>
       </c>
       <c r="I3">
-        <v>23.866176447391744</v>
+        <v>11.715853656867665</v>
+      </c>
+      <c r="J3">
+        <v>1.0141777360050148</v>
+      </c>
+      <c r="K3">
+        <v>38.84840735065351</v>
+      </c>
+      <c r="L3">
+        <v>23.277590695310806</v>
+      </c>
+      <c r="M3">
+        <v>116.47353178631496</v>
+      </c>
+      <c r="N3">
+        <v>34.811568463568335</v>
+      </c>
+      <c r="O3">
+        <v>10.147704164784699</v>
+      </c>
+      <c r="P3">
+        <v>32.643688089241856</v>
+      </c>
+      <c r="Q3">
+        <v>5.1609111854629521</v>
+      </c>
+      <c r="R3">
+        <v>20.812053037658316</v>
+      </c>
+      <c r="S3">
+        <v>16.388113959583489</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.35933783316164253</v>
+        <v>0.26698111766955995</v>
       </c>
       <c r="B4">
-        <v>20.372935049446575</v>
+        <v>39274.013348111286</v>
       </c>
       <c r="C4">
-        <v>18.624112795831529</v>
+        <v>0.29774150721407944</v>
       </c>
       <c r="D4">
-        <v>33.314135015728112</v>
+        <v>33.390806589551822</v>
       </c>
       <c r="E4">
-        <v>35.177546386489475</v>
+        <v>12738920.171506403</v>
       </c>
       <c r="F4">
-        <v>28.096184267128709</v>
+        <v>14182975.825430201</v>
       </c>
       <c r="G4">
-        <v>29.10676961852668</v>
+        <v>14.03880466851562</v>
       </c>
       <c r="H4">
-        <v>30.806528017469848</v>
+        <v>43.206819882737427</v>
       </c>
       <c r="I4">
-        <v>23.551261448561682</v>
-      </c>
-      <c r="L4" s="25"/>
+        <v>9.9525069786968974</v>
+      </c>
+      <c r="J4">
+        <v>0.48228789072402922</v>
+      </c>
+      <c r="K4">
+        <v>45.241875502440102</v>
+      </c>
+      <c r="L4" s="25">
+        <v>41.63305266191491</v>
+      </c>
+      <c r="M4">
+        <v>276.74217753538369</v>
+      </c>
+      <c r="N4">
+        <v>35.359440679528277</v>
+      </c>
+      <c r="O4">
+        <v>65535</v>
+      </c>
+      <c r="P4">
+        <v>31.962756249979922</v>
+      </c>
+      <c r="Q4">
+        <v>3.4118064406572564</v>
+      </c>
+      <c r="R4">
+        <v>23.866176447391744</v>
+      </c>
+      <c r="S4">
+        <v>15.377687775050815</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.34387364708602081</v>
+        <v>0.35933783316164253</v>
       </c>
       <c r="B5">
-        <v>77.369606165605788</v>
+        <v>64026.44107621452</v>
       </c>
       <c r="C5">
-        <v>62.363966507937029</v>
+        <v>0.2196960007178472</v>
       </c>
       <c r="D5">
-        <v>43.443566400056703</v>
+        <v>20.372935049446575</v>
       </c>
       <c r="E5">
-        <v>51.712553908003869</v>
+        <v>11660815.389813524</v>
       </c>
       <c r="F5">
-        <v>26.791796370902254</v>
+        <v>15746001.233835166</v>
       </c>
       <c r="G5">
-        <v>51.744233499347608</v>
+        <v>18.624112795831529</v>
       </c>
       <c r="H5">
-        <v>43.34296430768245</v>
+        <v>33.314135015728112</v>
       </c>
       <c r="I5">
-        <v>33.465758842333642</v>
+        <v>8.3248995491209179</v>
+      </c>
+      <c r="J5">
+        <v>0.62146782257943423</v>
+      </c>
+      <c r="K5">
+        <v>35.177546386489475</v>
+      </c>
+      <c r="L5">
+        <v>28.096184267128709</v>
+      </c>
+      <c r="M5">
+        <v>131.99859525068348</v>
+      </c>
+      <c r="N5">
+        <v>29.10676961852668</v>
+      </c>
+      <c r="O5">
+        <v>149551654.81536677</v>
       </c>
       <c r="P5" s="39">
-        <v>0.68029399999999995</v>
+        <v>30.806528017469848</v>
       </c>
       <c r="Q5" s="39">
-        <v>14.36734</v>
+        <v>4.3379828015827844</v>
       </c>
       <c r="R5" s="39">
-        <v>53.357640000000004</v>
+        <v>23.551261448561682</v>
       </c>
       <c r="S5" s="39">
-        <v>24.927990000000001</v>
+        <v>13.278955923320112</v>
       </c>
       <c r="T5" s="39">
         <v>27.509250000000002</v>
@@ -8910,43 +9017,61 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.33506683054146424</v>
+        <v>0.34387364708602081</v>
       </c>
       <c r="B6">
-        <v>60.174042250514447</v>
+        <v>9147441664.3559856</v>
       </c>
       <c r="C6">
-        <v>70.772994369132917</v>
+        <v>0.16127039307728611</v>
       </c>
       <c r="D6">
-        <v>33.197199515206243</v>
+        <v>77.369606165605788</v>
       </c>
       <c r="E6">
-        <v>41.144595726212735</v>
+        <v>1.9290048029375352E+18</v>
       </c>
       <c r="F6">
-        <v>18.926217222075252</v>
+        <v>2.801819736520597E+18</v>
       </c>
       <c r="G6">
-        <v>42.521834635580191</v>
+        <v>62.363966507937029</v>
       </c>
       <c r="H6">
-        <v>37.450196851082339</v>
+        <v>43.443566400056703</v>
       </c>
       <c r="I6">
-        <v>27.08994181247148</v>
+        <v>19.802115942320338</v>
+      </c>
+      <c r="J6">
+        <v>1.4626982397490671</v>
+      </c>
+      <c r="K6">
+        <v>51.712553908003869</v>
+      </c>
+      <c r="L6">
+        <v>26.791796370902254</v>
+      </c>
+      <c r="M6">
+        <v>141.35315939797886</v>
+      </c>
+      <c r="N6">
+        <v>51.744233499347608</v>
+      </c>
+      <c r="O6">
+        <v>18.279787512399285</v>
       </c>
       <c r="P6" s="39">
-        <v>0.31323899999999999</v>
+        <v>43.34296430768245</v>
       </c>
       <c r="Q6" s="39">
-        <v>24.631589999999999</v>
+        <v>7.3080205694117195</v>
       </c>
       <c r="R6" s="39">
-        <v>32.5351</v>
+        <v>33.465758842333642</v>
       </c>
       <c r="S6" s="39">
-        <v>25.22383</v>
+        <v>24.85729790564373</v>
       </c>
       <c r="T6" s="39">
         <v>29.80743</v>
@@ -8966,43 +9091,61 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.45280611092443795</v>
+        <v>0.33506683054146424</v>
       </c>
       <c r="B7">
-        <v>27.460498428617271</v>
+        <v>621158150.54461765</v>
       </c>
       <c r="C7">
-        <v>35.458238134848095</v>
+        <v>0.10442477316346464</v>
       </c>
       <c r="D7">
-        <v>35.26734159215561</v>
+        <v>60.174042250514447</v>
       </c>
       <c r="E7">
-        <v>39.998500617030622</v>
+        <v>2.2739472572257246E+20</v>
       </c>
       <c r="F7">
-        <v>25.0441175460994</v>
+        <v>3.6764427167066312E+20</v>
       </c>
       <c r="G7">
-        <v>35.320773438636586</v>
+        <v>70.772994369132917</v>
       </c>
       <c r="H7">
-        <v>37.394201405106315</v>
+        <v>33.197199515206243</v>
       </c>
       <c r="I7">
-        <v>28.194582095621172</v>
+        <v>17.026340576566227</v>
+      </c>
+      <c r="J7">
+        <v>1.6960669498047289</v>
+      </c>
+      <c r="K7">
+        <v>41.144595726212735</v>
+      </c>
+      <c r="L7">
+        <v>18.926217222075252</v>
+      </c>
+      <c r="M7">
+        <v>84.482643114858618</v>
+      </c>
+      <c r="N7">
+        <v>42.521834635580191</v>
+      </c>
+      <c r="O7">
+        <v>1.3901698702784904</v>
       </c>
       <c r="P7" s="39">
-        <v>0.26703500000000002</v>
+        <v>37.450196851082339</v>
       </c>
       <c r="Q7" s="39">
-        <v>11.671760000000001</v>
+        <v>7.4357658243047737</v>
       </c>
       <c r="R7" s="39">
-        <v>14.04162</v>
+        <v>27.08994181247148</v>
       </c>
       <c r="S7" s="39">
-        <v>20.40061</v>
+        <v>21.067085368232753</v>
       </c>
       <c r="T7" s="39">
         <v>21.494890000000002</v>
@@ -9021,17 +9164,62 @@
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.45280611092443795</v>
+      </c>
+      <c r="B8">
+        <v>2723227.9512344319</v>
+      </c>
+      <c r="C8">
+        <v>0.17333530579880232</v>
+      </c>
+      <c r="D8">
+        <v>27.460498428617271</v>
+      </c>
+      <c r="E8">
+        <v>7078511204.2171917</v>
+      </c>
+      <c r="F8">
+        <v>10784896704.219383</v>
+      </c>
+      <c r="G8">
+        <v>35.458238134848095</v>
+      </c>
+      <c r="H8">
+        <v>35.26734159215561</v>
+      </c>
+      <c r="I8">
+        <v>11.227535573950105</v>
+      </c>
+      <c r="J8">
+        <v>1.0291592446967921</v>
+      </c>
+      <c r="K8">
+        <v>39.998500617030622</v>
+      </c>
+      <c r="L8">
+        <v>25.0441175460994</v>
+      </c>
+      <c r="M8">
+        <v>103.21750311087098</v>
+      </c>
+      <c r="N8">
+        <v>35.320773438636586</v>
+      </c>
+      <c r="O8">
+        <v>-6.9202824218865526</v>
+      </c>
       <c r="P8" s="39">
-        <v>0.35930200000000001</v>
+        <v>37.394201405106315</v>
       </c>
       <c r="Q8" s="39">
-        <v>4.2178009999999997</v>
+        <v>6.422533260982461</v>
       </c>
       <c r="R8" s="39">
-        <v>18.622250000000001</v>
+        <v>28.194582095621172</v>
       </c>
       <c r="S8" s="39">
-        <v>10.8209</v>
+        <v>16.791435597158287</v>
       </c>
       <c r="T8" s="39">
         <v>10.4069</v>
@@ -9050,17 +9238,62 @@
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="P9" s="39">
-        <v>0.34387400000000001</v>
-      </c>
-      <c r="Q9" s="39">
-        <v>7.9991050000000001</v>
-      </c>
-      <c r="R9" s="39">
-        <v>62.363979999999998</v>
-      </c>
-      <c r="S9" s="39">
-        <v>8.5952439999999992</v>
+      <c r="A9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P9" s="39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q9" s="39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R9" s="39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S9" s="39" t="e">
+        <v>#N/A</v>
       </c>
       <c r="T9" s="39">
         <v>11.201169999999999</v>
@@ -9782,15 +10015,15 @@
     </row>
     <row r="28" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="45"/>
-      <c r="G28" s="102" t="s">
+      <c r="G28" s="111" t="s">
         <v>84</v>
       </c>
-      <c r="H28" s="103"/>
-      <c r="I28" s="103"/>
-      <c r="J28" s="103"/>
-      <c r="K28" s="103"/>
-      <c r="L28" s="103"/>
-      <c r="M28" s="104"/>
+      <c r="H28" s="112"/>
+      <c r="I28" s="112"/>
+      <c r="J28" s="112"/>
+      <c r="K28" s="112"/>
+      <c r="L28" s="112"/>
+      <c r="M28" s="113"/>
     </row>
     <row r="29" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F29" s="46" t="s">

</xml_diff>